<commit_message>
added code to do rand from adc on start
</commit_message>
<xml_diff>
--- a/Assembly_BoM.xlsx
+++ b/Assembly_BoM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\My Documents\Google Drive\Shitty Add-Ons\i-fucking-love-fucking-you\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA123D12-9A1E-4E4A-80B0-9B6D5E2B509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D625141-4EA7-412D-9DC9-7319528FDF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{967376A9-4158-458E-B93A-5370EC25A0FB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="91">
   <si>
     <t>*Ref Des</t>
   </si>
@@ -265,18 +265,9 @@
     <t>Microchip ATTiny10 microcontroller</t>
   </si>
   <si>
-    <t>https://lcsc.com/product-detail/MOSFETs_UMW-Youtai-Semiconductor-Co-Ltd-AO3404A_C347497.html</t>
-  </si>
-  <si>
-    <t>AO3404A</t>
-  </si>
-  <si>
     <t>SOT-23</t>
   </si>
   <si>
-    <t>n-channel mosfet</t>
-  </si>
-  <si>
     <t>https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_CCTC-TCC0603X7R104K500CT_C282519.html</t>
   </si>
   <si>
@@ -293,13 +284,37 @@
   </si>
   <si>
     <t>68 Ohm resistor</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Bipolar-Transistors-BJT_PANJIT-International-MMBT2222A_C2992465.html</t>
+  </si>
+  <si>
+    <t>npn bjt transistor</t>
+  </si>
+  <si>
+    <t>MMBT2222A</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJPA3J102V_C441891.html</t>
+  </si>
+  <si>
+    <t>ERJPA3J102V</t>
+  </si>
+  <si>
+    <t>1k Ohm resistor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +373,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -403,10 +426,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -426,18 +450,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,8 +467,22 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,64 +496,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>17780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>16510</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B15C13-2EB5-4AF2-8210-DADC91928BA3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="193040"/>
-          <a:ext cx="2241550" cy="627380"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -827,16 +795,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138196C9-4FCB-48B9-B05E-1EA800664D30}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="3" width="32.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="12" customWidth="1"/>
     <col min="5" max="8" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -847,29 +815,29 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="13.8">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
@@ -879,37 +847,37 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" s="15" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="18" t="s">
         <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E7" t="s">
@@ -926,7 +894,7 @@
       <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E8" t="s">
@@ -943,7 +911,7 @@
       <c r="C9" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E9" t="s">
@@ -960,7 +928,7 @@
       <c r="C10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E10" t="s">
@@ -977,7 +945,7 @@
       <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E11" t="s">
@@ -994,7 +962,7 @@
       <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E12" t="s">
@@ -1011,7 +979,7 @@
       <c r="C13" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E13" t="s">
@@ -1028,7 +996,7 @@
       <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E14" t="s">
@@ -1045,7 +1013,7 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E15" t="s">
@@ -1062,7 +1030,7 @@
       <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E16" t="s">
@@ -1079,7 +1047,7 @@
       <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E17" t="s">
@@ -1096,7 +1064,7 @@
       <c r="C18" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E18" t="s">
@@ -1113,7 +1081,7 @@
       <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E19" t="s">
@@ -1130,7 +1098,7 @@
       <c r="C20" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E20" t="s">
@@ -1147,7 +1115,7 @@
       <c r="C21" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E21" t="s">
@@ -1164,7 +1132,7 @@
       <c r="C22" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E22" t="s">
@@ -1181,7 +1149,7 @@
       <c r="C23" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E23" t="s">
@@ -1198,7 +1166,7 @@
       <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E24" t="s">
@@ -1215,7 +1183,7 @@
       <c r="C25" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E25" t="s">
@@ -1232,7 +1200,7 @@
       <c r="C26" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E26" t="s">
@@ -1249,7 +1217,7 @@
       <c r="C27" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E27" t="s">
@@ -1266,7 +1234,7 @@
       <c r="C28" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E28" t="s">
@@ -1283,7 +1251,7 @@
       <c r="C29" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E29" t="s">
@@ -1300,7 +1268,7 @@
       <c r="C30" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E30" t="s">
@@ -1317,7 +1285,7 @@
       <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E31" t="s">
@@ -1334,7 +1302,7 @@
       <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E32" t="s">
@@ -1351,7 +1319,7 @@
       <c r="C33" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E33" t="s">
@@ -1368,7 +1336,7 @@
       <c r="C34" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E34" t="s">
@@ -1385,7 +1353,7 @@
       <c r="C35" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E35" t="s">
@@ -1402,7 +1370,7 @@
       <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E36" t="s">
@@ -1419,7 +1387,7 @@
       <c r="C37" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E37" t="s">
@@ -1436,7 +1404,7 @@
       <c r="C38" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E38" t="s">
@@ -1453,7 +1421,7 @@
       <c r="C39" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E39" t="s">
@@ -1470,7 +1438,7 @@
       <c r="C40" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E40" t="s">
@@ -1487,7 +1455,7 @@
       <c r="C41" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E41" t="s">
@@ -1504,7 +1472,7 @@
       <c r="C42" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E42" t="s">
@@ -1521,7 +1489,7 @@
       <c r="C43" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E43" t="s">
@@ -1538,7 +1506,7 @@
       <c r="C44" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E44" t="s">
@@ -1555,7 +1523,7 @@
       <c r="C45" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E45" t="s">
@@ -1572,7 +1540,7 @@
       <c r="C46" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E46" t="s">
@@ -1589,7 +1557,7 @@
       <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E47" t="s">
@@ -1606,7 +1574,7 @@
       <c r="C48" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E48" t="s">
@@ -1623,7 +1591,7 @@
       <c r="C49" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E49" t="s">
@@ -1640,7 +1608,7 @@
       <c r="C50" t="s">
         <v>69</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E50" t="s">
@@ -1657,7 +1625,7 @@
       <c r="C51" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E51" t="s">
@@ -1674,7 +1642,7 @@
       <c r="C52" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E52" t="s">
@@ -1691,7 +1659,7 @@
       <c r="C53" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E53" t="s">
@@ -1708,7 +1676,7 @@
       <c r="C54" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E54" t="s">
@@ -1725,7 +1693,7 @@
       <c r="C55" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E55" t="s">
@@ -1742,7 +1710,7 @@
       <c r="C56" t="s">
         <v>69</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E56" t="s">
@@ -1759,7 +1727,7 @@
       <c r="C57" t="s">
         <v>69</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E57" t="s">
@@ -1776,7 +1744,7 @@
       <c r="C58" t="s">
         <v>69</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E58" t="s">
@@ -1793,7 +1761,7 @@
       <c r="C59" t="s">
         <v>69</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E59" t="s">
@@ -1810,7 +1778,7 @@
       <c r="C60" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E60" t="s">
@@ -1827,7 +1795,7 @@
       <c r="C61" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E61" t="s">
@@ -1844,7 +1812,7 @@
       <c r="C62" t="s">
         <v>69</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E62" t="s">
@@ -1856,16 +1824,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C63" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E63" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1873,16 +1841,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D64" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E64" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1890,16 +1858,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
-      </c>
-      <c r="D65" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1907,66 +1875,100 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>84</v>
-      </c>
-      <c r="D66" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>71</v>
       </c>
       <c r="E66" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C67" t="s">
-        <v>77</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="E67" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>78</v>
+        <v>89</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="E68" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>85</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
         <v>66</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C71" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D71" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E71" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1976,8 +1978,10 @@
     <mergeCell ref="C2:E4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{99A9E6DB-1124-4969-871E-B53FDC468CD1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>